<commit_message>
Added animations and other value textbox
</commit_message>
<xml_diff>
--- a/dist/files/ficheiro.xlsx
+++ b/dist/files/ficheiro.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="151">
   <si>
     <t>Data</t>
   </si>
@@ -100,7 +100,10 @@
     <t>Indique o seu nível de conhecimento sobre as associações empresariais e institutos de apoio à atividade empreendedora na Região Autónoma da Madeira (RAM).Instituto de Emprego da Madeira, IP-RAM</t>
   </si>
   <si>
-    <t>Indique o seu nível de conhecimento sobre as associações empresariais e institutos de apoio à atividade empreendedora na Região Autónoma da Madeira (RAM).Outra. Qual?</t>
+    <t>Indique o seu nível de conhecimento sobre as associações empresariais e institutos de apoio à atividade empreendedora na Região Autónoma da Madeira (RAM).Outra</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de conhecimento sobre as associações empresariais e institutos de apoio à atividade empreendedora na Região Autónoma da Madeira (RAM).Outro</t>
   </si>
   <si>
     <t>Para cada uma das seguintes medidas de apoio à criação de empresas na RAM, indique o seu nível de conhecimento.Treino específico para jovens empreendedores</t>
@@ -121,7 +124,10 @@
     <t>Para cada uma das seguintes medidas de apoio à criação de empresas na RAM, indique o seu nível de conhecimento.Serviços de consultoria em condições favoráveis</t>
   </si>
   <si>
-    <t>Para cada uma das seguintes medidas de apoio à criação de empresas na RAM, indique o seu nível de conhecimento.Outra. Qual?</t>
+    <t>Para cada uma das seguintes medidas de apoio à criação de empresas na RAM, indique o seu nível de conhecimento.Outra</t>
+  </si>
+  <si>
+    <t>Para cada uma das seguintes medidas de apoio à criação de empresas na RAM, indique o seu nível de conhecimento.Outro</t>
   </si>
   <si>
     <t>O que gostaria de fazer logo que acabe(ou) o seu curso?.Trabalhar por conta de outrém/assalariado/dependente</t>
@@ -148,6 +154,9 @@
     <t>No médio e longo prazo, considerando todas as vantagens e desvantagens (económicas, pessoais, reconhecimento social, estabilidade laboral, entre outros), indique o seu nível de atração em relação a cada uma das seguintes opções profissionais.Outra</t>
   </si>
   <si>
+    <t>No médio e longo prazo, considerando todas as vantagens e desvantagens (económicas, pessoais, reconhecimento social, estabilidade laboral, entre outros), indique o seu nível de atração em relação a cada uma das seguintes opções profissionais.Outro</t>
+  </si>
+  <si>
     <t>Indique o seu nível de concordância com as seguintes afirmações 1.Para mim, ser empreendedor traz mais vantagens do que desvantagens</t>
   </si>
   <si>
@@ -202,15 +211,15 @@
     <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Estou preparado para começar uma empresa viável</t>
   </si>
   <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Consigo controlar o processo da criação de uma empresa</t>
+  </si>
+  <si>
     <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Conheço os detalhes práticos necessários para começar uma empresa</t>
   </si>
   <si>
     <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Sei como desenvolver um projeto empreendedor</t>
   </si>
   <si>
-    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Consigo controlar o processo da criação de uma empresa</t>
-  </si>
-  <si>
     <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Se eu tentar criar uma empresa, teria uma elevada probabilidade de fazê-lo com sucesso</t>
   </si>
   <si>
@@ -337,10 +346,67 @@
     <t>Numa fase posterior serão selecionados alguns inqueridos para um estudo mais aprofundado. Pretende participar nesse estudo?</t>
   </si>
   <si>
+    <t>Antes de 2010</t>
+  </si>
+  <si>
+    <t>Menos de 22</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Solteiro(a)</t>
+  </si>
+  <si>
+    <t>Trabalhador independente</t>
+  </si>
+  <si>
+    <t>menos de 1 ano</t>
+  </si>
+  <si>
+    <t>Licenciatura</t>
+  </si>
+  <si>
+    <t>Ciências da Engenharia e Tecnologia</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Ensino do 2º ou 3º ciclo</t>
+  </si>
+  <si>
+    <t>Empreendedora/Dona de empresa</t>
+  </si>
+  <si>
+    <t>Empreendedor/Dono de empresa</t>
+  </si>
+  <si>
+    <t>Fora de Portugal mas na Europa</t>
+  </si>
+  <si>
+    <t>Entre €500 a €999</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Trabalhador por conta própria (nenhum empregado)</t>
+  </si>
+  <si>
+    <t>noo@gmail.com</t>
+  </si>
+  <si>
     <t>2010</t>
   </si>
   <si>
-    <t>26-30</t>
+    <t>31-35</t>
   </si>
   <si>
     <t>Masculino</t>
@@ -349,43 +415,55 @@
     <t>Casado(a)/União de facto</t>
   </si>
   <si>
-    <t>Trabalhador independente</t>
+    <t>Desempregado</t>
+  </si>
+  <si>
+    <t>5 a 10 anos</t>
+  </si>
+  <si>
+    <t>Doutoramento</t>
+  </si>
+  <si>
+    <t>Ciências Agrárias</t>
+  </si>
+  <si>
+    <t>Ensino técnico-profissional</t>
+  </si>
+  <si>
+    <t>Ensino secundário</t>
+  </si>
+  <si>
+    <t>Desempregada</t>
+  </si>
+  <si>
+    <t>Fora da Europa</t>
+  </si>
+  <si>
+    <t>De €4.000 a €6.999</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>mais de 35</t>
   </si>
   <si>
     <t>1 a 2 anos</t>
   </si>
   <si>
-    <t>Licenciatura</t>
-  </si>
-  <si>
-    <t>Outra</t>
-  </si>
-  <si>
-    <t>Depois de 2019</t>
-  </si>
-  <si>
-    <t>Ensino do 2º ou 3º ciclo</t>
-  </si>
-  <si>
-    <t>Ensino secundário</t>
-  </si>
-  <si>
-    <t>Fora da Europa</t>
-  </si>
-  <si>
-    <t>Entre €500 a €999</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>Outro</t>
-  </si>
-  <si>
-    <t>Microempresa  (até 9 empregados)</t>
-  </si>
-  <si>
-    <t>xax@gmail.com</t>
+    <t>Mestrado</t>
+  </si>
+  <si>
+    <t>Ciências Médicas e da Saúde</t>
+  </si>
+  <si>
+    <t>ainda não terminou</t>
+  </si>
+  <si>
+    <t>Ensino universitário</t>
+  </si>
+  <si>
+    <t>iti</t>
   </si>
 </sst>
 </file>
@@ -767,13 +845,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DD2"/>
+  <dimension ref="A1:DG5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="108" width="10" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="111" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1098,331 +1177,1060 @@
       <c r="DD1" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="DE1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44637.61978883102</v>
+        <v>44642.603227997686</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R2" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" t="s">
+        <v>126</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>2</v>
+      </c>
+      <c r="AG2">
+        <v>2</v>
+      </c>
+      <c r="AH2">
+        <v>2</v>
+      </c>
+      <c r="AI2">
+        <v>2</v>
+      </c>
+      <c r="AJ2">
+        <v>2</v>
+      </c>
+      <c r="AK2">
+        <v>2</v>
+      </c>
+      <c r="AN2">
+        <v>2</v>
+      </c>
+      <c r="AO2">
+        <v>2</v>
+      </c>
+      <c r="AP2">
+        <v>2</v>
+      </c>
+      <c r="AQ2">
+        <v>2</v>
+      </c>
+      <c r="AR2">
+        <v>2</v>
+      </c>
+      <c r="AS2">
+        <v>2</v>
+      </c>
+      <c r="AT2">
+        <v>2</v>
+      </c>
+      <c r="AU2">
+        <v>6</v>
+      </c>
+      <c r="AW2">
+        <v>2</v>
+      </c>
+      <c r="AX2">
+        <v>2</v>
+      </c>
+      <c r="AY2">
+        <v>2</v>
+      </c>
+      <c r="AZ2">
+        <v>2</v>
+      </c>
+      <c r="BA2">
+        <v>2</v>
+      </c>
+      <c r="BB2">
+        <v>2</v>
+      </c>
+      <c r="BC2">
+        <v>2</v>
+      </c>
+      <c r="BD2">
+        <v>2</v>
+      </c>
+      <c r="BE2">
+        <v>2</v>
+      </c>
+      <c r="BF2">
+        <v>2</v>
+      </c>
+      <c r="BG2">
+        <v>5</v>
+      </c>
+      <c r="BH2">
+        <v>2</v>
+      </c>
+      <c r="BI2">
+        <v>2</v>
+      </c>
+      <c r="BJ2">
+        <v>2</v>
+      </c>
+      <c r="BK2">
+        <v>2</v>
+      </c>
+      <c r="BL2">
+        <v>2</v>
+      </c>
+      <c r="BM2">
+        <v>2</v>
+      </c>
+      <c r="BN2">
+        <v>2</v>
+      </c>
+      <c r="BO2">
+        <v>2</v>
+      </c>
+      <c r="BP2">
+        <v>2</v>
+      </c>
+      <c r="BQ2">
+        <v>2</v>
+      </c>
+      <c r="BR2">
+        <v>2</v>
+      </c>
+      <c r="BS2">
+        <v>2</v>
+      </c>
+      <c r="BT2">
+        <v>2</v>
+      </c>
+      <c r="BU2">
+        <v>2</v>
+      </c>
+      <c r="BV2">
+        <v>2</v>
+      </c>
+      <c r="BW2">
+        <v>2</v>
+      </c>
+      <c r="BX2">
+        <v>2</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BZ2">
+        <v>2</v>
+      </c>
+      <c r="CA2">
+        <v>2</v>
+      </c>
+      <c r="CB2">
+        <v>2</v>
+      </c>
+      <c r="CC2">
+        <v>2</v>
+      </c>
+      <c r="CD2">
+        <v>2</v>
+      </c>
+      <c r="CE2">
+        <v>2</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CG2">
+        <v>2</v>
+      </c>
+      <c r="CH2">
+        <v>2</v>
+      </c>
+      <c r="CI2">
+        <v>2</v>
+      </c>
+      <c r="CJ2">
+        <v>2</v>
+      </c>
+      <c r="CK2">
+        <v>2</v>
+      </c>
+      <c r="CL2">
+        <v>2</v>
+      </c>
+      <c r="CM2">
+        <v>3</v>
+      </c>
+      <c r="CN2">
+        <v>2</v>
+      </c>
+      <c r="CO2">
+        <v>2</v>
+      </c>
+      <c r="CP2">
+        <v>2</v>
+      </c>
+      <c r="CQ2">
+        <v>2</v>
+      </c>
+      <c r="CR2">
+        <v>2</v>
+      </c>
+      <c r="CS2">
+        <v>2</v>
+      </c>
+      <c r="CT2">
+        <v>2</v>
+      </c>
+      <c r="CU2">
+        <v>2</v>
+      </c>
+      <c r="CV2">
+        <v>2</v>
+      </c>
+      <c r="CW2">
+        <v>2</v>
+      </c>
+      <c r="CX2">
+        <v>2</v>
+      </c>
+      <c r="CY2">
+        <v>2</v>
+      </c>
+      <c r="CZ2">
+        <v>2</v>
+      </c>
+      <c r="DA2">
+        <v>5</v>
+      </c>
+      <c r="DB2">
+        <v>2</v>
+      </c>
+      <c r="DC2">
+        <v>2</v>
+      </c>
+      <c r="DD2">
+        <v>2</v>
+      </c>
+      <c r="DE2">
+        <v>2</v>
+      </c>
+      <c r="DF2">
+        <v>2</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44644.405670092594</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" t="s">
+        <v>142</v>
+      </c>
+      <c r="T3" t="s">
+        <v>125</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3">
+        <v>2</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3">
+        <v>2</v>
+      </c>
+      <c r="AH3">
+        <v>2</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+      <c r="AJ3">
+        <v>2</v>
+      </c>
+      <c r="AK3">
+        <v>2</v>
+      </c>
+      <c r="AL3">
+        <v>2</v>
+      </c>
+      <c r="AN3">
+        <v>2</v>
+      </c>
+      <c r="AO3">
+        <v>2</v>
+      </c>
+      <c r="AP3">
+        <v>2</v>
+      </c>
+      <c r="AQ3">
+        <v>2</v>
+      </c>
+      <c r="AR3">
+        <v>2</v>
+      </c>
+      <c r="AS3">
+        <v>2</v>
+      </c>
+      <c r="AT3">
+        <v>2</v>
+      </c>
+      <c r="AU3">
+        <v>2</v>
+      </c>
+      <c r="AW3">
+        <v>2</v>
+      </c>
+      <c r="AX3">
+        <v>2</v>
+      </c>
+      <c r="AY3">
+        <v>2</v>
+      </c>
+      <c r="AZ3">
+        <v>2</v>
+      </c>
+      <c r="BA3">
+        <v>2</v>
+      </c>
+      <c r="BB3">
+        <v>2</v>
+      </c>
+      <c r="BC3">
+        <v>2</v>
+      </c>
+      <c r="BD3">
+        <v>2</v>
+      </c>
+      <c r="BE3">
+        <v>2</v>
+      </c>
+      <c r="BF3">
+        <v>2</v>
+      </c>
+      <c r="BG3">
+        <v>2</v>
+      </c>
+      <c r="BH3">
+        <v>2</v>
+      </c>
+      <c r="BI3">
+        <v>2</v>
+      </c>
+      <c r="BJ3">
+        <v>2</v>
+      </c>
+      <c r="BK3">
+        <v>2</v>
+      </c>
+      <c r="BL3">
+        <v>2</v>
+      </c>
+      <c r="BM3">
+        <v>2</v>
+      </c>
+      <c r="BN3">
+        <v>2</v>
+      </c>
+      <c r="BO3">
+        <v>2</v>
+      </c>
+      <c r="BP3">
+        <v>2</v>
+      </c>
+      <c r="BQ3">
+        <v>2</v>
+      </c>
+      <c r="BR3">
+        <v>2</v>
+      </c>
+      <c r="BS3">
+        <v>2</v>
+      </c>
+      <c r="BT3">
+        <v>2</v>
+      </c>
+      <c r="BU3">
+        <v>2</v>
+      </c>
+      <c r="BV3">
+        <v>2</v>
+      </c>
+      <c r="BW3">
+        <v>2</v>
+      </c>
+      <c r="BX3">
+        <v>2</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BZ3">
+        <v>2</v>
+      </c>
+      <c r="CA3">
+        <v>2</v>
+      </c>
+      <c r="CB3">
+        <v>2</v>
+      </c>
+      <c r="CC3">
+        <v>2</v>
+      </c>
+      <c r="CD3">
+        <v>2</v>
+      </c>
+      <c r="CE3">
+        <v>2</v>
+      </c>
+      <c r="CW3">
+        <v>2</v>
+      </c>
+      <c r="CX3">
+        <v>2</v>
+      </c>
+      <c r="CY3">
+        <v>2</v>
+      </c>
+      <c r="CZ3">
+        <v>2</v>
+      </c>
+      <c r="DA3">
+        <v>2</v>
+      </c>
+      <c r="DB3">
+        <v>2</v>
+      </c>
+      <c r="DC3">
+        <v>2</v>
+      </c>
+      <c r="DD3">
+        <v>2</v>
+      </c>
+      <c r="DE3">
+        <v>2</v>
+      </c>
+      <c r="DF3">
+        <v>2</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44644.5984609838</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AF4">
+        <v>2</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4">
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+      <c r="AJ4">
+        <v>2</v>
+      </c>
+      <c r="AK4">
+        <v>2</v>
+      </c>
+      <c r="AN4">
+        <v>2</v>
+      </c>
+      <c r="AO4">
+        <v>2</v>
+      </c>
+      <c r="AP4">
+        <v>2</v>
+      </c>
+      <c r="AQ4">
+        <v>2</v>
+      </c>
+      <c r="AR4">
+        <v>2</v>
+      </c>
+      <c r="AS4">
+        <v>2</v>
+      </c>
+      <c r="AT4">
+        <v>2</v>
+      </c>
+      <c r="AW4">
+        <v>2</v>
+      </c>
+      <c r="AX4">
+        <v>2</v>
+      </c>
+      <c r="AY4">
+        <v>2</v>
+      </c>
+      <c r="AZ4">
+        <v>2</v>
+      </c>
+      <c r="BA4">
+        <v>2</v>
+      </c>
+      <c r="BB4">
+        <v>2</v>
+      </c>
+      <c r="BC4">
+        <v>2</v>
+      </c>
+      <c r="BD4">
+        <v>2</v>
+      </c>
+      <c r="BE4">
+        <v>2</v>
+      </c>
+      <c r="BF4">
+        <v>2</v>
+      </c>
+      <c r="BG4">
+        <v>2</v>
+      </c>
+      <c r="BH4">
+        <v>2</v>
+      </c>
+      <c r="BI4">
+        <v>2</v>
+      </c>
+      <c r="BJ4">
+        <v>2</v>
+      </c>
+      <c r="BK4">
+        <v>2</v>
+      </c>
+      <c r="BL4">
+        <v>2</v>
+      </c>
+      <c r="BM4">
+        <v>2</v>
+      </c>
+      <c r="BN4">
+        <v>2</v>
+      </c>
+      <c r="BO4">
+        <v>2</v>
+      </c>
+      <c r="BP4">
+        <v>2</v>
+      </c>
+      <c r="BQ4">
+        <v>2</v>
+      </c>
+      <c r="BR4">
+        <v>2</v>
+      </c>
+      <c r="BS4">
+        <v>2</v>
+      </c>
+      <c r="BT4">
+        <v>2</v>
+      </c>
+      <c r="BU4">
+        <v>2</v>
+      </c>
+      <c r="BV4">
+        <v>2</v>
+      </c>
+      <c r="BW4">
+        <v>2</v>
+      </c>
+      <c r="BX4">
+        <v>2</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BZ4">
+        <v>2</v>
+      </c>
+      <c r="CA4">
+        <v>2</v>
+      </c>
+      <c r="CB4">
+        <v>2</v>
+      </c>
+      <c r="CC4">
+        <v>2</v>
+      </c>
+      <c r="CD4">
+        <v>1</v>
+      </c>
+      <c r="CE4">
+        <v>2</v>
+      </c>
+      <c r="CW4">
+        <v>2</v>
+      </c>
+      <c r="CX4">
+        <v>2</v>
+      </c>
+      <c r="CY4">
+        <v>2</v>
+      </c>
+      <c r="CZ4">
+        <v>2</v>
+      </c>
+      <c r="DA4">
+        <v>2</v>
+      </c>
+      <c r="DB4">
+        <v>2</v>
+      </c>
+      <c r="DC4">
+        <v>2</v>
+      </c>
+      <c r="DD4">
+        <v>2</v>
+      </c>
+      <c r="DE4">
+        <v>2</v>
+      </c>
+      <c r="DF4">
+        <v>2</v>
+      </c>
+      <c r="DG4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44650.63155788195</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
         <v>114</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F5" t="s">
         <v>115</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N2" t="s">
-        <v>117</v>
-      </c>
-      <c r="O2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>115</v>
-      </c>
-      <c r="R2" t="s">
-        <v>119</v>
-      </c>
-      <c r="S2" t="s">
-        <v>120</v>
-      </c>
-      <c r="T2" t="s">
-        <v>121</v>
-      </c>
-      <c r="U2" t="s">
-        <v>122</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2">
-        <v>2</v>
-      </c>
-      <c r="X2">
-        <v>2</v>
-      </c>
-      <c r="Y2">
-        <v>2</v>
-      </c>
-      <c r="Z2">
-        <v>2</v>
-      </c>
-      <c r="AA2">
-        <v>2</v>
-      </c>
-      <c r="AB2">
-        <v>2</v>
-      </c>
-      <c r="AC2">
-        <v>3</v>
-      </c>
-      <c r="AD2">
-        <v>5</v>
-      </c>
-      <c r="AE2">
-        <v>4</v>
-      </c>
-      <c r="AF2">
-        <v>5</v>
-      </c>
-      <c r="AG2">
-        <v>3</v>
-      </c>
-      <c r="AH2">
-        <v>4</v>
-      </c>
-      <c r="AI2">
-        <v>4</v>
-      </c>
-      <c r="AJ2">
+      <c r="G5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>148</v>
+      </c>
+      <c r="N5" t="s">
+        <v>149</v>
+      </c>
+      <c r="O5" t="s">
+        <v>138</v>
+      </c>
+      <c r="P5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" t="s">
+        <v>123</v>
+      </c>
+      <c r="S5" t="s">
+        <v>124</v>
+      </c>
+      <c r="T5" t="s">
+        <v>125</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>2</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>2</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF5">
+        <v>2</v>
+      </c>
+      <c r="AG5">
+        <v>2</v>
+      </c>
+      <c r="AH5">
+        <v>2</v>
+      </c>
+      <c r="AI5">
+        <v>2</v>
+      </c>
+      <c r="AJ5">
+        <v>2</v>
+      </c>
+      <c r="AK5">
+        <v>2</v>
+      </c>
+      <c r="AN5">
+        <v>2</v>
+      </c>
+      <c r="AO5">
+        <v>2</v>
+      </c>
+      <c r="AP5">
+        <v>2</v>
+      </c>
+      <c r="AQ5">
+        <v>2</v>
+      </c>
+      <c r="AR5">
+        <v>2</v>
+      </c>
+      <c r="AS5">
+        <v>2</v>
+      </c>
+      <c r="AT5">
+        <v>2</v>
+      </c>
+      <c r="AU5">
+        <v>2</v>
+      </c>
+      <c r="AW5">
+        <v>2</v>
+      </c>
+      <c r="AX5">
+        <v>2</v>
+      </c>
+      <c r="AY5">
+        <v>2</v>
+      </c>
+      <c r="AZ5">
+        <v>2</v>
+      </c>
+      <c r="BA5">
+        <v>2</v>
+      </c>
+      <c r="BB5">
+        <v>2</v>
+      </c>
+      <c r="BC5">
+        <v>2</v>
+      </c>
+      <c r="BD5">
+        <v>2</v>
+      </c>
+      <c r="BE5">
+        <v>2</v>
+      </c>
+      <c r="BF5">
+        <v>2</v>
+      </c>
+      <c r="BG5">
+        <v>2</v>
+      </c>
+      <c r="BH5">
+        <v>2</v>
+      </c>
+      <c r="BI5">
+        <v>2</v>
+      </c>
+      <c r="BJ5">
+        <v>2</v>
+      </c>
+      <c r="BK5">
+        <v>2</v>
+      </c>
+      <c r="BL5">
+        <v>2</v>
+      </c>
+      <c r="BM5">
+        <v>2</v>
+      </c>
+      <c r="BN5">
+        <v>2</v>
+      </c>
+      <c r="BO5">
+        <v>2</v>
+      </c>
+      <c r="BP5">
+        <v>2</v>
+      </c>
+      <c r="BQ5">
         <v>7</v>
       </c>
-      <c r="AK2">
-        <v>3</v>
-      </c>
-      <c r="AL2">
-        <v>2</v>
-      </c>
-      <c r="AM2">
-        <v>4</v>
-      </c>
-      <c r="AN2">
-        <v>2</v>
-      </c>
-      <c r="AO2">
-        <v>5</v>
-      </c>
-      <c r="AP2">
-        <v>4</v>
-      </c>
-      <c r="AQ2">
-        <v>2</v>
-      </c>
-      <c r="AR2">
-        <v>4</v>
-      </c>
-      <c r="AS2">
-        <v>4</v>
-      </c>
-      <c r="AT2">
-        <v>2</v>
-      </c>
-      <c r="AU2">
-        <v>2</v>
-      </c>
-      <c r="AV2">
-        <v>2</v>
-      </c>
-      <c r="AW2">
-        <v>3</v>
-      </c>
-      <c r="AX2">
-        <v>3</v>
-      </c>
-      <c r="AY2">
-        <v>2</v>
-      </c>
-      <c r="AZ2">
-        <v>3</v>
-      </c>
-      <c r="BA2">
-        <v>4</v>
-      </c>
-      <c r="BB2">
-        <v>3</v>
-      </c>
-      <c r="BC2">
-        <v>3</v>
-      </c>
-      <c r="BD2">
-        <v>5</v>
-      </c>
-      <c r="BE2">
-        <v>2</v>
-      </c>
-      <c r="BF2">
-        <v>3</v>
-      </c>
-      <c r="BG2">
-        <v>3</v>
-      </c>
-      <c r="BH2">
-        <v>4</v>
-      </c>
-      <c r="BI2">
-        <v>5</v>
-      </c>
-      <c r="BJ2">
-        <v>3</v>
-      </c>
-      <c r="BK2">
-        <v>3</v>
-      </c>
-      <c r="BL2">
-        <v>5</v>
-      </c>
-      <c r="BM2">
+      <c r="BR5">
+        <v>2</v>
+      </c>
+      <c r="BS5">
+        <v>2</v>
+      </c>
+      <c r="BT5">
+        <v>2</v>
+      </c>
+      <c r="BU5">
+        <v>2</v>
+      </c>
+      <c r="BV5">
+        <v>2</v>
+      </c>
+      <c r="BW5">
         <v>6</v>
       </c>
-      <c r="BN2">
-        <v>5</v>
-      </c>
-      <c r="BO2">
-        <v>3</v>
-      </c>
-      <c r="BP2">
-        <v>3</v>
-      </c>
-      <c r="BQ2">
-        <v>4</v>
-      </c>
-      <c r="BR2">
-        <v>4</v>
-      </c>
-      <c r="BS2">
-        <v>4</v>
-      </c>
-      <c r="BT2">
-        <v>6</v>
-      </c>
-      <c r="BU2">
-        <v>7</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BW2">
-        <v>2</v>
-      </c>
-      <c r="BX2">
-        <v>3</v>
-      </c>
-      <c r="BY2">
-        <v>4</v>
-      </c>
-      <c r="BZ2">
-        <v>1</v>
-      </c>
-      <c r="CA2">
-        <v>6</v>
-      </c>
-      <c r="CB2">
-        <v>7</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>123</v>
-      </c>
-      <c r="CD2">
-        <v>2</v>
-      </c>
-      <c r="CE2">
-        <v>3</v>
-      </c>
-      <c r="CF2">
-        <v>4</v>
-      </c>
-      <c r="CG2">
-        <v>5</v>
-      </c>
-      <c r="CH2">
-        <v>6</v>
-      </c>
-      <c r="CI2">
-        <v>7</v>
-      </c>
-      <c r="CJ2">
-        <v>2</v>
-      </c>
-      <c r="CK2">
-        <v>4</v>
-      </c>
-      <c r="CL2">
-        <v>6</v>
-      </c>
-      <c r="CM2">
-        <v>2</v>
-      </c>
-      <c r="CN2">
-        <v>3</v>
-      </c>
-      <c r="CO2">
-        <v>4</v>
-      </c>
-      <c r="CP2">
-        <v>7</v>
-      </c>
-      <c r="CQ2">
-        <v>5</v>
-      </c>
-      <c r="CR2">
-        <v>2</v>
-      </c>
-      <c r="CS2">
-        <v>4</v>
-      </c>
-      <c r="CT2">
-        <v>6</v>
-      </c>
-      <c r="CU2">
-        <v>5</v>
-      </c>
-      <c r="CV2">
-        <v>5</v>
-      </c>
-      <c r="CW2">
-        <v>3</v>
-      </c>
-      <c r="CX2">
-        <v>4</v>
-      </c>
-      <c r="CY2">
-        <v>2</v>
-      </c>
-      <c r="CZ2">
-        <v>4</v>
-      </c>
-      <c r="DA2">
-        <v>3</v>
-      </c>
-      <c r="DB2">
-        <v>5</v>
-      </c>
-      <c r="DC2">
-        <v>3</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>124</v>
+      <c r="BX5">
+        <v>2</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>125</v>
+      </c>
+      <c r="BZ5">
+        <v>2</v>
+      </c>
+      <c r="CA5">
+        <v>2</v>
+      </c>
+      <c r="CB5">
+        <v>2</v>
+      </c>
+      <c r="CC5">
+        <v>2</v>
+      </c>
+      <c r="CD5">
+        <v>2</v>
+      </c>
+      <c r="CE5">
+        <v>2</v>
+      </c>
+      <c r="CW5">
+        <v>2</v>
+      </c>
+      <c r="CX5">
+        <v>2</v>
+      </c>
+      <c r="CY5">
+        <v>2</v>
+      </c>
+      <c r="CZ5">
+        <v>2</v>
+      </c>
+      <c r="DA5">
+        <v>2</v>
+      </c>
+      <c r="DB5">
+        <v>2</v>
+      </c>
+      <c r="DC5">
+        <v>2</v>
+      </c>
+      <c r="DD5">
+        <v>2</v>
+      </c>
+      <c r="DE5">
+        <v>2</v>
+      </c>
+      <c r="DF5">
+        <v>2</v>
+      </c>
+      <c r="DG5" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alteracoes dia 06 Maio
</commit_message>
<xml_diff>
--- a/dist/files/ficheiro.xlsx
+++ b/dist/files/ficheiro.xlsx
@@ -11,14 +11,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="164">
   <si>
     <t>Data</t>
   </si>
   <si>
-    <t>Em que ano participou no Curso Intensivo em Empreendedorismo e Inovação Empresarial RS4E?</t>
-  </si>
-  <si>
     <t>Idade</t>
   </si>
   <si>
@@ -31,12 +28,6 @@
     <t>Situação laboral</t>
   </si>
   <si>
-    <t>Teste - empreendedor</t>
-  </si>
-  <si>
-    <t>Teste - não empreendedor</t>
-  </si>
-  <si>
     <t>Há quantos anos criou a empresa?</t>
   </si>
   <si>
@@ -88,28 +79,28 @@
     <t>Conhece pessoalmente algum empreendedor?</t>
   </si>
   <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Família.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Família.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Amigos.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Amigos.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Patrão.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Patrão.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Outro.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
-  </si>
-  <si>
-    <t>Indique qual a relação que tem com esse empreendor(a).Outro.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
+    <t>Qual a relação que tem com esse empreendor(a)?.Família.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Família.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Amigos.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Amigos.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Patrão.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Patrão.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Outro.Em que medida você conhece a atividade dele(a) como empreendedor(a)?</t>
+  </si>
+  <si>
+    <t>Qual a relação que tem com esse empreendor(a)?.Outro.Em que medida ele/ela pode ser considerado(a) um bom empreendedor(a)?</t>
   </si>
   <si>
     <t>Indique o seu nível de conhecimento sobre as associações empresariais e institutos de apoio à atividade empreendedora na RAM.StartUp Madeira</t>
@@ -217,6 +208,15 @@
     <t>Quando decidiu criar a sua empresa, as pessoas próximas de si aprovaram essa decisão?.Os seus colegas e companheiros</t>
   </si>
   <si>
+    <t>Se decidir criar uma empresa, as pessoas próximas de si aprovariam dessa decisão?.A sua família próxima</t>
+  </si>
+  <si>
+    <t>Se decidir criar uma empresa, as pessoas próximas de si aprovariam dessa decisão?.Os seus amigos</t>
+  </si>
+  <si>
+    <t>Se decidir criar uma empresa, as pessoas próximas de si aprovariam dessa decisão?.Os seus colegas e companheiros</t>
+  </si>
+  <si>
     <t>Indique o seu nível de concordância com as seguintes afirmações 2.A atividade empreendedora entra em choque com a cultura do meu país</t>
   </si>
   <si>
@@ -250,6 +250,24 @@
     <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Estou a ter sucesso com a minha empresa</t>
   </si>
   <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Criar uma empresa e mantê-la em funcionamento seria uma tarefa fácil para mim</t>
+  </si>
+  <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Estou preparado para começar uma empresa viável</t>
+  </si>
+  <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Consigo controlar o processo de criação de uma empresa</t>
+  </si>
+  <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Conheço os detalhes práticos necessários para começar uma empresa</t>
+  </si>
+  <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Sei como desenvolver um projeto empreendedor</t>
+  </si>
+  <si>
+    <t>Em que medida concorda com as seguintes afirmações sobre a sua capacidade empreendedora?.Se tentasse criar uma empresa, teria uma elevada probabilidade de fazê-lo com sucesso</t>
+  </si>
+  <si>
     <t>Analisando as capacidades necessárias para se ser empreendedor, você considera que:.Consegue reconhecer uma oportunidade empreendedora</t>
   </si>
   <si>
@@ -268,6 +286,60 @@
     <t>Analisando as capacidades necessárias para se ser empreendedor, você considera que:.Tem capacidade de networking e para realizar contactos profissionais</t>
   </si>
   <si>
+    <t>Já pensou seriamente em se tornar empreendedor e criar uma empresa?</t>
+  </si>
+  <si>
+    <t>Se criar uma empresa, qual a dimensão, em número de empregados, que gostaria de atingir?</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Ser competitivo em mercados internacionais</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Alcançar níveis altos de rendimentos</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Desenvolver o tipo de atividade que realmente gosta/aprecia</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Alcançar grande reconhecimento na sociedade</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Ajudar a resolver problemas na minha comunidade</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Manter o negócio/empresa a funcionar</t>
+  </si>
+  <si>
+    <t>Em que medida considera os seguintes resultados como reflexo de sucesso na atividade empreendedora?.Manter a empresa numa trajetória de crescimento</t>
+  </si>
+  <si>
+    <t>O quanto importante será para si o contínuo desenvolvimento da empresa?</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Exportar uma parte significativa da produção</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Apresentar, com regularidade, novos produtos e/ou serviços aos seus clientes</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Introduzir, com regularidade, novos processos ou sistemas de produção</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Desenvolver projectos de Pesquisa &amp; Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Planear detalhadamente as diferentes áreas de atuação da empresa</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Estabelecer acordos de cooperação e parcerias com outras empresas</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Oferecer formação especializada aos funcionários</t>
+  </si>
+  <si>
+    <t>Em que medida realizaria os seguintes comportamentos/ações para poder desenvolver a sua empresa?.Aumentar a dimensao da empresa (funcionários, instalações, …)</t>
+  </si>
+  <si>
     <t>Qual a dimensão, em número de empregados, que gostaria de atingir com a sua empresa?</t>
   </si>
   <si>
@@ -319,6 +391,24 @@
     <t>Em que medida realizaria os seguintes comportamentos/ações para fazer crescer a sua empresa?.Aumentar a dimensao da empresa (funcionários, instalações, etc, …)</t>
   </si>
   <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.Estou pronto para fazer qualquer coisa para me tornar empreendedor</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.O meu objetivo profissional é tornar-me um empreendedor</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.Vou fazer todo o esforço para criar e gerir a minha própria empresa</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.Estou determinado em criar uma empresa no futuro</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.Já pensei seriamente em criar uma empresa</t>
+  </si>
+  <si>
+    <t>Indique o seu nível de concordância com as seguintes afirmações:.Tenho a firme intenção de criar uma empresa algum dia</t>
+  </si>
+  <si>
     <t>Em que medida considera que é possível oferecer cursos de educação para o empreendedorismo que consigam desenvolver os seguintes aspetos?.Conhecimento sobre o ambiente empreendedor</t>
   </si>
   <si>
@@ -334,37 +424,85 @@
     <t>Em que medida considera que é possível oferecer cursos de educação para o empreendedorismo que consigam desenvolver os seguintes aspetos?.A intenção de ser empreendedor</t>
   </si>
   <si>
-    <t>Em que medida a sua participar no Curso de Empreendedorismo e Inovação Empresarial RS4E ajudou-o(a) a desenvolver os seguintes aspeto?.Conhecimento sobre o ambiente empreendedor</t>
-  </si>
-  <si>
-    <t>Em que medida a sua participar no Curso de Empreendedorismo e Inovação Empresarial RS4E ajudou-o(a) a desenvolver os seguintes aspeto?.Grande reconhecimento/apreço da figura do empreendedor</t>
-  </si>
-  <si>
-    <t>Em que medida a sua participar no Curso de Empreendedorismo e Inovação Empresarial RS4E ajudou-o(a) a desenvolver os seguintes aspeto?.A preferência por ser empreendedor</t>
-  </si>
-  <si>
-    <t>Em que medida a sua participar no Curso de Empreendedorismo e Inovação Empresarial RS4E ajudou-o(a) a desenvolver os seguintes aspeto?.As habilidades/capacidades necessárias para se ser empreendedor</t>
-  </si>
-  <si>
-    <t>Em que medida a sua participar no Curso de Empreendedorismo e Inovação Empresarial RS4E ajudou-o(a) a desenvolver os seguintes aspeto?.A intenção de ser empreendedor</t>
+    <t>Participou em algum curso/módulo que possa ser considerado educação para o empreendedorismo?</t>
+  </si>
+  <si>
+    <t>Se sim, em que medida ajudou-o(a) a desenvolver os seguintes aspetos?.Conhecimento sobre o ambiente empreendedor</t>
+  </si>
+  <si>
+    <t>Se sim, em que medida ajudou-o(a) a desenvolver os seguintes aspetos?.Grande reconhecimento/apreço da figura do empreendedor</t>
+  </si>
+  <si>
+    <t>Se sim, em que medida ajudou-o(a) a desenvolver os seguintes aspetos?.A preferência por ser empreendedor</t>
+  </si>
+  <si>
+    <t>Se sim, em que medida ajudou-o(a) a desenvolver os seguintes aspetos?.As habilidades/capacidades necessárias para se ser empreendedor</t>
+  </si>
+  <si>
+    <t>Se sim, em que medida ajudou-o(a) a desenvolver os seguintes aspetos?.A intenção de ser empreendedor</t>
   </si>
   <si>
     <t>Numa fase posterior serão selecionados alguns inqueridos para um estudo mais aprofundado. Pretende participar nesse estudo?</t>
   </si>
   <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>chato@gmail.com</t>
-  </si>
-  <si>
-    <t>De €2.000 a €3.999</t>
-  </si>
-  <si>
-    <t>Trabalhador por conta própria (nenhum empregado)</t>
-  </si>
-  <si>
-    <t>cam@hotmail.com</t>
+    <t>Menos de 22</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Solteiro(a)</t>
+  </si>
+  <si>
+    <t>Trabalhador por conta de outrém</t>
+  </si>
+  <si>
+    <t>Menos de 1 ano</t>
+  </si>
+  <si>
+    <t>Mestrado</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>31-35</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>Divorciado(a)</t>
+  </si>
+  <si>
+    <t>Reformado</t>
+  </si>
+  <si>
+    <t>5 a 10 anos</t>
+  </si>
+  <si>
+    <t>Doutoramento</t>
+  </si>
+  <si>
+    <t>26-30</t>
+  </si>
+  <si>
+    <t>Casado(a)/União de facto</t>
+  </si>
+  <si>
+    <t>Empreendedor/Dono de empresa</t>
+  </si>
+  <si>
+    <t>3 a 5 anos</t>
+  </si>
+  <si>
+    <t>Outros serviços</t>
+  </si>
+  <si>
+    <t>mais de 10 anos</t>
+  </si>
+  <si>
+    <t>Pós-doutoramento</t>
   </si>
 </sst>
 </file>
@@ -746,14 +884,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI4"/>
+  <dimension ref="A1:EN4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="113" width="10" customWidth="1"/>
+    <col min="2" max="144" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:144" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1093,284 +1231,182 @@
       <c r="DI1" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="DJ1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44684.5898053125</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z2">
-        <v>3</v>
-      </c>
-      <c r="AA2">
-        <v>4</v>
-      </c>
-      <c r="AB2">
-        <v>2</v>
-      </c>
-      <c r="AC2">
-        <v>3</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>2</v>
-      </c>
-      <c r="AF2">
-        <v>7</v>
-      </c>
-      <c r="AG2">
-        <v>7</v>
+        <v>44690.63788592593</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
+        <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>44684.606900729166</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>113</v>
-      </c>
-      <c r="DI3" t="s">
-        <v>114</v>
+        <v>44690.63820667824</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" t="s">
+        <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>44686.38161287037</v>
-      </c>
-      <c r="X4" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z4">
-        <v>6</v>
-      </c>
-      <c r="AA4">
-        <v>6</v>
-      </c>
-      <c r="AD4">
-        <v>6</v>
-      </c>
-      <c r="AE4">
-        <v>4</v>
-      </c>
-      <c r="AH4">
-        <v>6</v>
-      </c>
-      <c r="AI4">
-        <v>5</v>
-      </c>
-      <c r="AJ4">
-        <v>5</v>
-      </c>
-      <c r="AK4">
-        <v>5</v>
-      </c>
-      <c r="AL4">
-        <v>5</v>
-      </c>
-      <c r="AO4">
-        <v>4</v>
-      </c>
-      <c r="AP4">
-        <v>3</v>
-      </c>
-      <c r="AQ4">
-        <v>1</v>
-      </c>
-      <c r="AR4">
-        <v>4</v>
-      </c>
-      <c r="AS4">
-        <v>6</v>
-      </c>
-      <c r="AT4">
-        <v>4</v>
-      </c>
-      <c r="AW4">
-        <v>5</v>
-      </c>
-      <c r="AX4">
-        <v>3</v>
-      </c>
-      <c r="AY4">
-        <v>3</v>
-      </c>
-      <c r="AZ4">
-        <v>6</v>
-      </c>
-      <c r="BA4">
-        <v>3</v>
-      </c>
-      <c r="BB4">
-        <v>5</v>
-      </c>
-      <c r="BC4">
-        <v>5</v>
-      </c>
-      <c r="BF4">
-        <v>4</v>
-      </c>
-      <c r="BG4">
-        <v>4</v>
-      </c>
-      <c r="BH4">
-        <v>5</v>
-      </c>
-      <c r="BI4">
-        <v>5</v>
-      </c>
-      <c r="BJ4">
-        <v>4</v>
-      </c>
-      <c r="BK4">
-        <v>3</v>
-      </c>
-      <c r="BL4">
-        <v>5</v>
-      </c>
-      <c r="BM4">
-        <v>5</v>
-      </c>
-      <c r="BQ4">
-        <v>4</v>
-      </c>
-      <c r="BR4">
-        <v>5</v>
-      </c>
-      <c r="BS4">
-        <v>3</v>
-      </c>
-      <c r="BT4">
-        <v>5</v>
-      </c>
-      <c r="BU4">
-        <v>4</v>
-      </c>
-      <c r="BV4">
-        <v>4</v>
-      </c>
-      <c r="BW4">
-        <v>3</v>
-      </c>
-      <c r="BX4">
-        <v>4</v>
-      </c>
-      <c r="BY4">
-        <v>4</v>
-      </c>
-      <c r="BZ4">
-        <v>3</v>
-      </c>
-      <c r="CA4">
-        <v>3</v>
-      </c>
-      <c r="CB4">
-        <v>3</v>
-      </c>
-      <c r="CC4">
-        <v>5</v>
-      </c>
-      <c r="CD4">
-        <v>6</v>
-      </c>
-      <c r="CE4">
-        <v>5</v>
-      </c>
-      <c r="CF4">
-        <v>5</v>
-      </c>
-      <c r="CG4">
-        <v>5</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>116</v>
-      </c>
-      <c r="CI4">
-        <v>3</v>
-      </c>
-      <c r="CJ4">
-        <v>3</v>
-      </c>
-      <c r="CK4">
-        <v>3</v>
-      </c>
-      <c r="CL4">
-        <v>3</v>
-      </c>
-      <c r="CM4">
-        <v>3</v>
-      </c>
-      <c r="CN4">
-        <v>3</v>
-      </c>
-      <c r="CO4">
-        <v>3</v>
-      </c>
-      <c r="CP4">
-        <v>4</v>
-      </c>
-      <c r="CQ4">
-        <v>4</v>
-      </c>
-      <c r="CR4">
-        <v>4</v>
-      </c>
-      <c r="CS4">
-        <v>4</v>
-      </c>
-      <c r="CT4">
-        <v>4</v>
-      </c>
-      <c r="CU4">
-        <v>4</v>
-      </c>
-      <c r="CV4">
-        <v>4</v>
-      </c>
-      <c r="CW4">
-        <v>4</v>
-      </c>
-      <c r="CX4">
-        <v>4</v>
-      </c>
-      <c r="CY4">
-        <v>4</v>
-      </c>
-      <c r="CZ4">
-        <v>4</v>
-      </c>
-      <c r="DA4">
-        <v>3</v>
-      </c>
-      <c r="DB4">
-        <v>3</v>
-      </c>
-      <c r="DC4">
-        <v>4</v>
-      </c>
-      <c r="DD4">
-        <v>4</v>
-      </c>
-      <c r="DE4">
-        <v>4</v>
-      </c>
-      <c r="DF4">
-        <v>4</v>
-      </c>
-      <c r="DG4">
-        <v>4</v>
-      </c>
-      <c r="DH4">
-        <v>4</v>
-      </c>
-      <c r="DI4" t="s">
-        <v>117</v>
+        <v>44690.64042167824</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>